<commit_message>
energy carrier price updates for historic and future scenario simulations
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_EnergyCarrier_EmissionFactor.xlsx
+++ b/projects/test_building/input/Scenario_EnergyCarrier_EmissionFactor.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670DBE6E-90B5-6E42-AA84-C6BB21F40F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="30240" windowHeight="17385"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -177,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -656,55 +655,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AT28" totalsRowShown="0">
-  <autoFilter ref="A1:AT28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AT28" totalsRowShown="0">
+  <autoFilter ref="A1:AT28"/>
   <tableColumns count="46">
-    <tableColumn id="6" xr3:uid="{9352D49A-984B-8F43-88AC-058CF01CD45A}" name="id_scenario"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="id_region"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_energy_carrier" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="unit" dataDxfId="42"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="2010" dataDxfId="41"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="2011" dataDxfId="40"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="2012" dataDxfId="39"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="2013" dataDxfId="38"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="2014" dataDxfId="37"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="2015" dataDxfId="36"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="2016" dataDxfId="35"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="2017" dataDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="2018" dataDxfId="33"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="2019" dataDxfId="32"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="2020" dataDxfId="31"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="2021" dataDxfId="30"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="2022" dataDxfId="29"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="2023" dataDxfId="28"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="2024" dataDxfId="27"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="2025" dataDxfId="26"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="2026" dataDxfId="25"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="2027" dataDxfId="24"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="2028" dataDxfId="23"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="2029" dataDxfId="22"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="2030" dataDxfId="21"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="2031" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="2032" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="2033" dataDxfId="18"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="2034" dataDxfId="17"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="2035" dataDxfId="16"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="2036" dataDxfId="15"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="2037" dataDxfId="14"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="2038" dataDxfId="13"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="2039" dataDxfId="12"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="2040" dataDxfId="11"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="2041" dataDxfId="10"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="2042" dataDxfId="9"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="2043" dataDxfId="8"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="2044" dataDxfId="7"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="2045" dataDxfId="6"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="2046" dataDxfId="5"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="2047" dataDxfId="4"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="2048" dataDxfId="3"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="2049" dataDxfId="2"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="2050" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{14B6D2E0-C275-F244-8EFF-D0B358220AB3}" name="2051" dataDxfId="0"/>
+    <tableColumn id="6" name="id_scenario"/>
+    <tableColumn id="3" name="id_region"/>
+    <tableColumn id="1" name="id_energy_carrier" dataDxfId="43"/>
+    <tableColumn id="4" name="unit" dataDxfId="42"/>
+    <tableColumn id="16" name="2010" dataDxfId="41"/>
+    <tableColumn id="17" name="2011" dataDxfId="40"/>
+    <tableColumn id="18" name="2012" dataDxfId="39"/>
+    <tableColumn id="19" name="2013" dataDxfId="38"/>
+    <tableColumn id="20" name="2014" dataDxfId="37"/>
+    <tableColumn id="21" name="2015" dataDxfId="36"/>
+    <tableColumn id="22" name="2016" dataDxfId="35"/>
+    <tableColumn id="23" name="2017" dataDxfId="34"/>
+    <tableColumn id="24" name="2018" dataDxfId="33"/>
+    <tableColumn id="25" name="2019" dataDxfId="32"/>
+    <tableColumn id="26" name="2020" dataDxfId="31"/>
+    <tableColumn id="27" name="2021" dataDxfId="30"/>
+    <tableColumn id="28" name="2022" dataDxfId="29"/>
+    <tableColumn id="29" name="2023" dataDxfId="28"/>
+    <tableColumn id="30" name="2024" dataDxfId="27"/>
+    <tableColumn id="31" name="2025" dataDxfId="26"/>
+    <tableColumn id="32" name="2026" dataDxfId="25"/>
+    <tableColumn id="33" name="2027" dataDxfId="24"/>
+    <tableColumn id="34" name="2028" dataDxfId="23"/>
+    <tableColumn id="35" name="2029" dataDxfId="22"/>
+    <tableColumn id="36" name="2030" dataDxfId="21"/>
+    <tableColumn id="37" name="2031" dataDxfId="20"/>
+    <tableColumn id="2" name="2032" dataDxfId="19"/>
+    <tableColumn id="5" name="2033" dataDxfId="18"/>
+    <tableColumn id="38" name="2034" dataDxfId="17"/>
+    <tableColumn id="39" name="2035" dataDxfId="16"/>
+    <tableColumn id="40" name="2036" dataDxfId="15"/>
+    <tableColumn id="41" name="2037" dataDxfId="14"/>
+    <tableColumn id="42" name="2038" dataDxfId="13"/>
+    <tableColumn id="43" name="2039" dataDxfId="12"/>
+    <tableColumn id="44" name="2040" dataDxfId="11"/>
+    <tableColumn id="45" name="2041" dataDxfId="10"/>
+    <tableColumn id="46" name="2042" dataDxfId="9"/>
+    <tableColumn id="47" name="2043" dataDxfId="8"/>
+    <tableColumn id="48" name="2044" dataDxfId="7"/>
+    <tableColumn id="49" name="2045" dataDxfId="6"/>
+    <tableColumn id="50" name="2046" dataDxfId="5"/>
+    <tableColumn id="51" name="2047" dataDxfId="4"/>
+    <tableColumn id="52" name="2048" dataDxfId="3"/>
+    <tableColumn id="53" name="2049" dataDxfId="2"/>
+    <tableColumn id="54" name="2050" dataDxfId="1"/>
+    <tableColumn id="7" name="2051" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -972,20 +971,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AW18" sqref="AW18"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="46" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="46" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -2822,130 +2821,130 @@
         <v>44</v>
       </c>
       <c r="E14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="J14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="K14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="L14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="M14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="P14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="S14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="T14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="U14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="V14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="W14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="X14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AH14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AI14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AJ14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AK14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AM14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AN14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AO14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AP14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AQ14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AR14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AS14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
       <c r="AT14" s="2">
-        <v>3.0959999975231997E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:46">

</xml_diff>